<commit_message>
after data from user
</commit_message>
<xml_diff>
--- a/pidsg25.xlsx
+++ b/pidsg25.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="p1normal" sheetId="1" state="visible" r:id="rId3"/>
@@ -734,11 +734,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="84104289"/>
-        <c:axId val="81719343"/>
+        <c:axId val="71878431"/>
+        <c:axId val="93589215"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="84104289"/>
+        <c:axId val="71878431"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,7 +770,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81719343"/>
+        <c:crossAx val="93589215"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -778,7 +778,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81719343"/>
+        <c:axId val="93589215"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -817,7 +817,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84104289"/>
+        <c:crossAx val="71878431"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -970,11 +970,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="18274129"/>
-        <c:axId val="29122159"/>
+        <c:axId val="48377999"/>
+        <c:axId val="66291658"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="18274129"/>
+        <c:axId val="48377999"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1006,7 +1006,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29122159"/>
+        <c:crossAx val="66291658"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1014,7 +1014,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29122159"/>
+        <c:axId val="66291658"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1053,7 +1053,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18274129"/>
+        <c:crossAx val="48377999"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1206,11 +1206,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="4770894"/>
-        <c:axId val="99011312"/>
+        <c:axId val="86369860"/>
+        <c:axId val="97981054"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="4770894"/>
+        <c:axId val="86369860"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1242,7 +1242,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99011312"/>
+        <c:crossAx val="97981054"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1250,7 +1250,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99011312"/>
+        <c:axId val="97981054"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1289,7 +1289,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4770894"/>
+        <c:crossAx val="86369860"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1442,11 +1442,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="32939322"/>
-        <c:axId val="8685786"/>
+        <c:axId val="16877994"/>
+        <c:axId val="99305741"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="32939322"/>
+        <c:axId val="16877994"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1478,7 +1478,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8685786"/>
+        <c:crossAx val="99305741"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1486,7 +1486,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8685786"/>
+        <c:axId val="99305741"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1525,7 +1525,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32939322"/>
+        <c:crossAx val="16877994"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1678,11 +1678,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="88091628"/>
-        <c:axId val="87012218"/>
+        <c:axId val="17023086"/>
+        <c:axId val="61805301"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88091628"/>
+        <c:axId val="17023086"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1714,7 +1714,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87012218"/>
+        <c:crossAx val="61805301"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1722,7 +1722,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87012218"/>
+        <c:axId val="61805301"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1761,7 +1761,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88091628"/>
+        <c:crossAx val="17023086"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1914,11 +1914,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="45786056"/>
-        <c:axId val="22786435"/>
+        <c:axId val="76055821"/>
+        <c:axId val="77829876"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="45786056"/>
+        <c:axId val="76055821"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1950,7 +1950,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22786435"/>
+        <c:crossAx val="77829876"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1958,7 +1958,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22786435"/>
+        <c:axId val="77829876"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1997,7 +1997,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45786056"/>
+        <c:crossAx val="76055821"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2150,11 +2150,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="65106617"/>
-        <c:axId val="69755538"/>
+        <c:axId val="47761050"/>
+        <c:axId val="30731236"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="65106617"/>
+        <c:axId val="47761050"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2186,7 +2186,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69755538"/>
+        <c:crossAx val="30731236"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2194,7 +2194,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69755538"/>
+        <c:axId val="30731236"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2233,7 +2233,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65106617"/>
+        <c:crossAx val="47761050"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2386,11 +2386,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="43126999"/>
-        <c:axId val="5111256"/>
+        <c:axId val="96070858"/>
+        <c:axId val="68324675"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43126999"/>
+        <c:axId val="96070858"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2422,7 +2422,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5111256"/>
+        <c:crossAx val="68324675"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2430,7 +2430,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5111256"/>
+        <c:axId val="68324675"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2469,7 +2469,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43126999"/>
+        <c:crossAx val="96070858"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2512,9 +2512,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>712800</xdr:colOff>
+      <xdr:colOff>712440</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>120240</xdr:rowOff>
+      <xdr:rowOff>119880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2523,7 +2523,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="398880" y="9380880"/>
-        <a:ext cx="4683960" cy="2931480"/>
+        <a:ext cx="4683600" cy="2931120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2542,9 +2542,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>323280</xdr:colOff>
+      <xdr:colOff>322920</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2553,7 +2553,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5153040" y="9389520"/>
-        <a:ext cx="4709160" cy="2931480"/>
+        <a:ext cx="4708800" cy="2931120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2572,9 +2572,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>704520</xdr:colOff>
+      <xdr:colOff>704160</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>120240</xdr:rowOff>
+      <xdr:rowOff>119880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2583,7 +2583,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="10034280" y="9380880"/>
-        <a:ext cx="4673160" cy="2931480"/>
+        <a:ext cx="4672800" cy="2931120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2602,9 +2602,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>712800</xdr:colOff>
+      <xdr:colOff>712440</xdr:colOff>
       <xdr:row>80</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2613,7 +2613,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="398880" y="12445920"/>
-        <a:ext cx="4683960" cy="2931120"/>
+        <a:ext cx="4683600" cy="2930760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2632,9 +2632,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>340560</xdr:colOff>
+      <xdr:colOff>340200</xdr:colOff>
       <xdr:row>80</xdr:row>
-      <xdr:rowOff>145800</xdr:rowOff>
+      <xdr:rowOff>145440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2643,7 +2643,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5170320" y="12454560"/>
-        <a:ext cx="4709160" cy="2931120"/>
+        <a:ext cx="4708800" cy="2930760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2662,9 +2662,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>704520</xdr:colOff>
+      <xdr:colOff>704160</xdr:colOff>
       <xdr:row>80</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2673,7 +2673,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="10034280" y="12445920"/>
-        <a:ext cx="4673160" cy="2931120"/>
+        <a:ext cx="4672800" cy="2930760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2692,9 +2692,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>55</xdr:col>
-      <xdr:colOff>221760</xdr:colOff>
+      <xdr:colOff>221400</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>103320</xdr:rowOff>
+      <xdr:rowOff>102960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2703,7 +2703,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="43478280" y="9554400"/>
-        <a:ext cx="4673160" cy="2931480"/>
+        <a:ext cx="4672800" cy="2931120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2722,9 +2722,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>86</xdr:col>
-      <xdr:colOff>255600</xdr:colOff>
+      <xdr:colOff>255240</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>27360</xdr:rowOff>
+      <xdr:rowOff>27000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2733,7 +2733,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="71189280" y="9847080"/>
-        <a:ext cx="4673160" cy="2943720"/>
+        <a:ext cx="4672800" cy="2943360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9447,7 +9447,7 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -10127,7 +10127,7 @@
   </sheetPr>
   <dimension ref="A1:CX49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>

</xml_diff>